<commit_message>
Rename sample form to an appropriate name/id
</commit_message>
<xml_diff>
--- a/extras/sample-form/Button to advance.xlsx
+++ b/extras/sample-form/Button to advance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/button-to-advance/extras/sample-form/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cking/github/button-to-advance/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98798DCE-A691-1147-9C1A-370F4438D67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59878F1D-8F5D-8A4A-A797-7BE427A24CF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26940" yWindow="680" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9660" yWindow="6480" windowWidth="28740" windowHeight="17520" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="help-choices" sheetId="5" r:id="rId5"/>
     <sheet name="help-settings" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -2597,12 +2597,6 @@
     <t>min=0.25;max=2</t>
   </si>
   <si>
-    <t>Form definition spreadsheet template</t>
-  </si>
-  <si>
-    <t>form_definition_spreadsheet_template</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -2634,6 +2628,12 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Sample form - button to advance</t>
+  </si>
+  <si>
+    <t>sample_form_button_to_advance</t>
   </si>
 </sst>
 </file>
@@ -4785,7 +4785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4990,13 +4990,13 @@
         <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="51" x14ac:dyDescent="0.2">
@@ -5004,16 +5004,16 @@
         <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>373</v>
-      </c>
       <c r="F13" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5021,10 +5021,10 @@
         <v>148</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="51" x14ac:dyDescent="0.2">
@@ -5032,10 +5032,10 @@
         <v>42</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -5293,8 +5293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5330,20 +5330,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008031908</v>
+        <v>2008041244</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Updated sample form name
</commit_message>
<xml_diff>
--- a/extras/sample-form/Button to advance.xlsx
+++ b/extras/sample-form/Button to advance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/button-to-advance/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98798DCE-A691-1147-9C1A-370F4438D67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0B8991-0BD3-1F4D-834E-843F9239E8D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26940" yWindow="680" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2480" yWindow="520" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2597,12 +2597,6 @@
     <t>min=0.25;max=2</t>
   </si>
   <si>
-    <t>Form definition spreadsheet template</t>
-  </si>
-  <si>
-    <t>form_definition_spreadsheet_template</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -2634,6 +2628,12 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Button to advance</t>
+  </si>
+  <si>
+    <t>button_to_advance</t>
   </si>
 </sst>
 </file>
@@ -4990,13 +4990,13 @@
         <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="51" x14ac:dyDescent="0.2">
@@ -5004,16 +5004,16 @@
         <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>373</v>
-      </c>
       <c r="F13" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5021,10 +5021,10 @@
         <v>148</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="51" x14ac:dyDescent="0.2">
@@ -5032,10 +5032,10 @@
         <v>42</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -5293,9 +5293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5330,20 +5328,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008031908</v>
+        <v>2008041322</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>29</v>

</xml_diff>